<commit_message>
very initial support for fa_3 format
</commit_message>
<xml_diff>
--- a/przykladowe-pliki-wejsciowe/przyklad.xlsx
+++ b/przykladowe-pliki-wejsciowe/przyklad.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="68">
   <si>
     <t xml:space="preserve">Sekcja</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t xml:space="preserve">00-111 Chmielowo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faktura.Podmiot2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GV</t>
   </si>
   <si>
     <t xml:space="preserve">Faktura.Fa.Platnosc</t>
@@ -231,6 +240,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -290,16 +300,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,264 +440,264 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G66" activeCellId="0" sqref="G66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>3333333333</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="3" t="n">
         <v>44562</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="3" t="n">
         <v>44563</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="0" t="n">
+      <c r="A23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="G23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>2222222222</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -691,7 +705,7 @@
       <c r="A33" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -699,334 +713,358 @@
       <c r="A34" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B39" s="3" t="n">
         <v>43831</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="0" t="s">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>44562</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>44563</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>4444444444</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="0" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B65" s="3" t="n">
+        <v>43831</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="0" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="D68" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="E68" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D69" s="1" t="n">
         <v>1.23</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E69" s="1" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="2" t="n">
-        <v>44562</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>44563</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="0" t="s">
+      <c r="G69" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="E70" s="1" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>4444444444</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B61" s="2" t="n">
-        <v>43831</v>
-      </c>
-      <c r="C61" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C65" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="D66" s="0" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="E66" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F66" s="0" t="n">
+      <c r="F70" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1035,8 +1073,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>